<commit_message>
NIAID Common Clinical Data Dictionary v1.5-Example.xlsx
</commit_message>
<xml_diff>
--- a/NIAID Common Clinical Data Dictionary v1.5-Example.xlsx
+++ b/NIAID Common Clinical Data Dictionary v1.5-Example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isingh/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isingh/GSCID-BRC-Project-and-Sample-Application-Standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="680" yWindow="2000" windowWidth="37480" windowHeight="19260"/>
+    <workbookView xWindow="-37980" yWindow="1100" windowWidth="37480" windowHeight="19260"/>
   </bookViews>
   <sheets>
     <sheet name="ICEMR" sheetId="6" r:id="rId1"/>
@@ -1844,9 +1844,6 @@
     <t>anemia</t>
   </si>
   <si>
-    <t>serve</t>
-  </si>
-  <si>
     <t xml:space="preserve">uninfected with malaria </t>
   </si>
   <si>
@@ -1896,6 +1893,9 @@
   </si>
   <si>
     <t>14.1 g/dL</t>
+  </si>
+  <si>
+    <t>severe</t>
   </si>
 </sst>
 </file>
@@ -2111,7 +2111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2263,6 +2263,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2567,8 +2568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3276,7 +3277,7 @@
         <v>595</v>
       </c>
       <c r="F6" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H6" s="43" t="s">
         <v>105</v>
@@ -3290,47 +3291,47 @@
       <c r="M6" s="45" t="s">
         <v>598</v>
       </c>
-      <c r="P6" s="45" t="s">
-        <v>599</v>
+      <c r="P6" s="53" t="s">
+        <v>616</v>
       </c>
       <c r="Q6" s="45" t="s">
+        <v>601</v>
+      </c>
+      <c r="S6" s="45" t="s">
+        <v>604</v>
+      </c>
+      <c r="T6" s="45" t="s">
         <v>602</v>
       </c>
-      <c r="S6" s="45" t="s">
+      <c r="U6" s="45" t="s">
+        <v>604</v>
+      </c>
+      <c r="V6" s="45" t="s">
         <v>605</v>
       </c>
-      <c r="T6" s="45" t="s">
+      <c r="W6" s="48" t="s">
+        <v>607</v>
+      </c>
+      <c r="X6" s="48" t="s">
         <v>603</v>
       </c>
-      <c r="U6" s="45" t="s">
-        <v>605</v>
-      </c>
-      <c r="V6" s="45" t="s">
-        <v>606</v>
-      </c>
-      <c r="W6" s="48" t="s">
+      <c r="Y6" s="48" t="s">
+        <v>607</v>
+      </c>
+      <c r="Z6" s="48" t="s">
+        <v>609</v>
+      </c>
+      <c r="AA6" s="48" t="s">
         <v>608</v>
       </c>
-      <c r="X6" s="48" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y6" s="48" t="s">
+      <c r="AB6" s="48" t="s">
+        <v>610</v>
+      </c>
+      <c r="AC6" s="48" t="s">
         <v>608</v>
       </c>
-      <c r="Z6" s="48" t="s">
-        <v>610</v>
-      </c>
-      <c r="AA6" s="48" t="s">
-        <v>609</v>
-      </c>
-      <c r="AB6" s="48" t="s">
+      <c r="AD6" s="45" t="s">
         <v>611</v>
-      </c>
-      <c r="AC6" s="48" t="s">
-        <v>609</v>
-      </c>
-      <c r="AD6" s="45" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="7" spans="1:44" ht="26" x14ac:dyDescent="0.15">
@@ -3352,43 +3353,43 @@
       <c r="M7" s="46"/>
       <c r="P7" s="46"/>
       <c r="Q7" s="46" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="S7" s="46" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T7" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="U7" s="46" t="s">
+        <v>604</v>
+      </c>
+      <c r="V7" s="46" t="s">
+        <v>606</v>
+      </c>
+      <c r="W7" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="X7" s="49" t="s">
         <v>603</v>
       </c>
-      <c r="U7" s="46" t="s">
-        <v>605</v>
-      </c>
-      <c r="V7" s="46" t="s">
+      <c r="Y7" s="49" t="s">
         <v>607</v>
-      </c>
-      <c r="W7" s="49" t="s">
-        <v>608</v>
-      </c>
-      <c r="X7" s="49" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y7" s="49" t="s">
-        <v>608</v>
       </c>
       <c r="Z7" s="49">
         <v>0</v>
       </c>
       <c r="AA7" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB7" s="49" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AC7" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD7" s="46" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="8" spans="1:44" ht="26" x14ac:dyDescent="0.15">
@@ -3410,43 +3411,43 @@
       <c r="M8" s="45"/>
       <c r="P8" s="45"/>
       <c r="Q8" s="45" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="S8" s="45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T8" s="45" t="s">
+        <v>602</v>
+      </c>
+      <c r="U8" s="45" t="s">
+        <v>604</v>
+      </c>
+      <c r="V8" s="45" t="s">
+        <v>606</v>
+      </c>
+      <c r="W8" s="48" t="s">
+        <v>607</v>
+      </c>
+      <c r="X8" s="48" t="s">
         <v>603</v>
       </c>
-      <c r="U8" s="45" t="s">
-        <v>605</v>
-      </c>
-      <c r="V8" s="45" t="s">
+      <c r="Y8" s="48" t="s">
         <v>607</v>
-      </c>
-      <c r="W8" s="48" t="s">
-        <v>608</v>
-      </c>
-      <c r="X8" s="48" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y8" s="48" t="s">
-        <v>608</v>
       </c>
       <c r="Z8" s="48">
         <v>0</v>
       </c>
       <c r="AA8" s="48" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB8" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AC8" s="48" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD8" s="45" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:44" ht="26" x14ac:dyDescent="0.15">
@@ -3468,43 +3469,43 @@
       <c r="M9" s="46"/>
       <c r="P9" s="46"/>
       <c r="Q9" s="46" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="S9" s="46" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T9" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="U9" s="46" t="s">
+        <v>604</v>
+      </c>
+      <c r="V9" s="46" t="s">
+        <v>606</v>
+      </c>
+      <c r="W9" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="X9" s="49" t="s">
         <v>603</v>
       </c>
-      <c r="U9" s="46" t="s">
-        <v>605</v>
-      </c>
-      <c r="V9" s="46" t="s">
+      <c r="Y9" s="49" t="s">
         <v>607</v>
-      </c>
-      <c r="W9" s="49" t="s">
-        <v>608</v>
-      </c>
-      <c r="X9" s="49" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y9" s="49" t="s">
-        <v>608</v>
       </c>
       <c r="Z9" s="49">
         <v>0</v>
       </c>
       <c r="AA9" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB9" s="49" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AC9" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD9" s="46" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="10" spans="1:44" ht="26" x14ac:dyDescent="0.15">
@@ -3526,44 +3527,44 @@
       <c r="M10" s="45"/>
       <c r="P10" s="45"/>
       <c r="Q10" s="45" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="R10" s="8"/>
       <c r="S10" s="45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T10" s="45" t="s">
+        <v>602</v>
+      </c>
+      <c r="U10" s="45" t="s">
+        <v>604</v>
+      </c>
+      <c r="V10" s="45" t="s">
+        <v>606</v>
+      </c>
+      <c r="W10" s="48" t="s">
+        <v>607</v>
+      </c>
+      <c r="X10" s="48" t="s">
         <v>603</v>
       </c>
-      <c r="U10" s="45" t="s">
-        <v>605</v>
-      </c>
-      <c r="V10" s="45" t="s">
+      <c r="Y10" s="48" t="s">
         <v>607</v>
-      </c>
-      <c r="W10" s="48" t="s">
-        <v>608</v>
-      </c>
-      <c r="X10" s="48" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y10" s="48" t="s">
-        <v>608</v>
       </c>
       <c r="Z10" s="48">
         <v>0</v>
       </c>
       <c r="AA10" s="48" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB10" s="48" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AC10" s="48" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD10" s="45" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="11" spans="1:44" ht="26" x14ac:dyDescent="0.15">
@@ -3585,44 +3586,44 @@
       <c r="M11" s="46"/>
       <c r="P11" s="46"/>
       <c r="Q11" s="46" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="46" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="T11" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="U11" s="46" t="s">
+        <v>604</v>
+      </c>
+      <c r="V11" s="46" t="s">
+        <v>606</v>
+      </c>
+      <c r="W11" s="49" t="s">
+        <v>607</v>
+      </c>
+      <c r="X11" s="49" t="s">
         <v>603</v>
       </c>
-      <c r="U11" s="46" t="s">
-        <v>605</v>
-      </c>
-      <c r="V11" s="46" t="s">
+      <c r="Y11" s="49" t="s">
         <v>607</v>
-      </c>
-      <c r="W11" s="49" t="s">
-        <v>608</v>
-      </c>
-      <c r="X11" s="49" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y11" s="49" t="s">
-        <v>608</v>
       </c>
       <c r="Z11" s="49">
         <v>0</v>
       </c>
       <c r="AA11" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AB11" s="49" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="AC11" s="49" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="AD11" s="46" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.15">

</xml_diff>